<commit_message>
Updates to Sprint Report.
</commit_message>
<xml_diff>
--- a/Team03Report.xlsx
+++ b/Team03Report.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
   <workbookPr date1904="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-20" windowWidth="14400" windowHeight="17460" tabRatio="819" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="-20" windowWidth="28800" windowHeight="17460" tabRatio="819" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="180">
   <si>
     <t>Initials</t>
   </si>
@@ -563,6 +563,9 @@
   </si>
   <si>
     <t>done</t>
+  </si>
+  <si>
+    <t>in progress</t>
   </si>
 </sst>
 </file>
@@ -629,7 +632,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -649,12 +652,16 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -812,11 +819,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2070634520"/>
-        <c:axId val="2128167592"/>
+        <c:axId val="2107844488"/>
+        <c:axId val="2107841208"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="2070634520"/>
+        <c:axId val="2107844488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -834,14 +841,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="2128167592"/>
+        <c:crossAx val="2107841208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="2128167592"/>
+        <c:axId val="2107841208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -869,7 +876,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="2070634520"/>
+        <c:crossAx val="2107844488"/>
         <c:crossesAt val="0.0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1343,11 +1350,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="5" max="5" width="18.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
@@ -1407,6 +1417,12 @@
       <c r="C4" t="s">
         <v>28</v>
       </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="5" spans="1:5">
       <c r="B5" t="s">
@@ -1415,6 +1431,12 @@
       <c r="C5" t="s">
         <v>30</v>
       </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6">
@@ -1457,6 +1479,12 @@
       <c r="C8" t="s">
         <v>36</v>
       </c>
+      <c r="D8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="9" spans="1:5">
       <c r="B9" t="s">
@@ -1464,6 +1492,12 @@
       </c>
       <c r="C9" t="s">
         <v>38</v>
+      </c>
+      <c r="D9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1545,7 +1579,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -1752,7 +1786,7 @@
       <c r="I14"/>
     </row>
     <row r="15" spans="1:9" ht="156">
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="11" t="s">
         <v>175</v>
       </c>
     </row>
@@ -1772,7 +1806,7 @@
       </c>
     </row>
     <row r="19" spans="2:2" ht="208">
-      <c r="B19" s="12" t="s">
+      <c r="B19" s="11" t="s">
         <v>176</v>
       </c>
     </row>
@@ -1787,7 +1821,7 @@
       </c>
     </row>
     <row r="22" spans="2:2" ht="169">
-      <c r="B22" s="12" t="s">
+      <c r="B22" s="11" t="s">
         <v>177</v>
       </c>
     </row>
@@ -1806,7 +1840,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -1956,485 +1990,487 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView topLeftCell="A13" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="3" max="3" width="8.7109375" style="3"/>
+    <col min="1" max="2" width="8.7109375" style="15"/>
+    <col min="3" max="3" width="8.7109375" style="16"/>
+    <col min="4" max="16384" width="8.7109375" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" ht="39">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" s="13" customFormat="1">
+      <c r="A1" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="14" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="255">
-      <c r="A2" t="s">
+    <row r="2" spans="1:3" ht="15">
+      <c r="A2" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="12" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="165">
-      <c r="A3" t="s">
+    <row r="3" spans="1:3" ht="15">
+      <c r="A3" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="12" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="150">
-      <c r="A4" t="s">
+    <row r="4" spans="1:3" ht="15">
+      <c r="A4" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="12" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="300">
-      <c r="A5" t="s">
+    <row r="5" spans="1:3" ht="15">
+      <c r="A5" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="12" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="195">
-      <c r="A6" t="s">
+    <row r="6" spans="1:3" ht="15">
+      <c r="A6" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="12" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="180">
-      <c r="A7" t="s">
+    <row r="7" spans="1:3" ht="15">
+      <c r="A7" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="12" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="409">
-      <c r="A8" t="s">
+    <row r="8" spans="1:3" ht="15">
+      <c r="A8" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="12" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="240">
-      <c r="A9" t="s">
+    <row r="9" spans="1:3" ht="15">
+      <c r="A9" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="12" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="300">
-      <c r="A10" t="s">
+    <row r="10" spans="1:3" ht="15">
+      <c r="A10" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="12" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="210">
-      <c r="A11" t="s">
+    <row r="11" spans="1:3" ht="15">
+      <c r="A11" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="12" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="210">
-      <c r="A12" t="s">
+    <row r="12" spans="1:3" ht="15">
+      <c r="A12" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="12" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="405">
-      <c r="A13" t="s">
+    <row r="13" spans="1:3" ht="15">
+      <c r="A13" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="12" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="285">
-      <c r="A14" t="s">
+    <row r="14" spans="1:3" ht="15">
+      <c r="A14" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="12" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="180">
-      <c r="A15" t="s">
+    <row r="15" spans="1:3" ht="15">
+      <c r="A15" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="C15" s="12" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="180">
-      <c r="A16" t="s">
+    <row r="16" spans="1:3" ht="15">
+      <c r="A16" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="12" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="210">
-      <c r="A17" t="s">
+    <row r="17" spans="1:3" ht="15">
+      <c r="A17" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="12" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="165">
-      <c r="A18" t="s">
+    <row r="18" spans="1:3" ht="15">
+      <c r="A18" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C18" s="12" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="120">
-      <c r="A19" t="s">
+    <row r="19" spans="1:3" ht="15">
+      <c r="A19" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="C19" s="11" t="s">
+      <c r="C19" s="12" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="135">
-      <c r="A20" t="s">
+    <row r="20" spans="1:3" ht="15">
+      <c r="A20" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="C20" s="12" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="195">
-      <c r="A21" t="s">
+    <row r="21" spans="1:3" ht="15">
+      <c r="A21" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="C21" s="12" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="255">
-      <c r="A22" t="s">
+    <row r="22" spans="1:3" ht="15">
+      <c r="A22" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="C22" s="12" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="225">
-      <c r="A23" t="s">
+    <row r="23" spans="1:3" ht="15">
+      <c r="A23" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="C23" s="11" t="s">
+      <c r="C23" s="12" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="315">
-      <c r="A24" t="s">
+    <row r="24" spans="1:3" ht="15">
+      <c r="A24" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="C24" s="11" t="s">
+      <c r="C24" s="12" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="390">
-      <c r="A25" t="s">
+    <row r="25" spans="1:3" ht="15">
+      <c r="A25" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="C25" s="11" t="s">
+      <c r="C25" s="12" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="285">
-      <c r="A26" t="s">
+    <row r="26" spans="1:3" ht="15">
+      <c r="A26" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="C26" s="11" t="s">
+      <c r="C26" s="12" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="409">
-      <c r="A27" t="s">
+    <row r="27" spans="1:3" ht="15">
+      <c r="A27" s="15" t="s">
         <v>125</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="15" t="s">
         <v>126</v>
       </c>
-      <c r="C27" s="11" t="s">
+      <c r="C27" s="12" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="180">
-      <c r="A28" t="s">
+    <row r="28" spans="1:3" ht="15">
+      <c r="A28" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="15" t="s">
         <v>128</v>
       </c>
-      <c r="C28" s="11" t="s">
+      <c r="C28" s="12" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="90">
-      <c r="A29" t="s">
+    <row r="29" spans="1:3" ht="15">
+      <c r="A29" s="15" t="s">
         <v>130</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="C29" s="11" t="s">
+      <c r="C29" s="12" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="150">
-      <c r="A30" t="s">
+    <row r="30" spans="1:3" ht="15">
+      <c r="A30" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="15" t="s">
         <v>134</v>
       </c>
-      <c r="C30" s="11" t="s">
+      <c r="C30" s="12" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="150">
-      <c r="A31" t="s">
+    <row r="31" spans="1:3" ht="15">
+      <c r="A31" s="15" t="s">
         <v>136</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="15" t="s">
         <v>137</v>
       </c>
-      <c r="C31" s="11" t="s">
+      <c r="C31" s="12" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="255">
-      <c r="A32" t="s">
+    <row r="32" spans="1:3" ht="15">
+      <c r="A32" s="15" t="s">
         <v>139</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="15" t="s">
         <v>140</v>
       </c>
-      <c r="C32" s="11" t="s">
+      <c r="C32" s="12" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="135">
-      <c r="A33" t="s">
+    <row r="33" spans="1:3" ht="15">
+      <c r="A33" s="15" t="s">
         <v>142</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="C33" s="11" t="s">
+      <c r="C33" s="12" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="285">
-      <c r="A34" t="s">
+    <row r="34" spans="1:3" ht="15">
+      <c r="A34" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="15" t="s">
         <v>146</v>
       </c>
-      <c r="C34" s="11" t="s">
+      <c r="C34" s="12" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="330">
-      <c r="A35" t="s">
+    <row r="35" spans="1:3" ht="15">
+      <c r="A35" s="15" t="s">
         <v>148</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="15" t="s">
         <v>149</v>
       </c>
-      <c r="C35" s="11" t="s">
+      <c r="C35" s="12" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="210">
-      <c r="A36" t="s">
+    <row r="36" spans="1:3" ht="15">
+      <c r="A36" s="15" t="s">
         <v>151</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="15" t="s">
         <v>152</v>
       </c>
-      <c r="C36" s="11" t="s">
+      <c r="C36" s="12" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="195">
-      <c r="A37" t="s">
+    <row r="37" spans="1:3" ht="15">
+      <c r="A37" s="15" t="s">
         <v>154</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="15" t="s">
         <v>155</v>
       </c>
-      <c r="C37" s="11" t="s">
+      <c r="C37" s="12" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="300">
-      <c r="A38" t="s">
+    <row r="38" spans="1:3" ht="15">
+      <c r="A38" s="15" t="s">
         <v>157</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="15" t="s">
         <v>158</v>
       </c>
-      <c r="C38" s="11" t="s">
+      <c r="C38" s="12" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="255">
-      <c r="A39" t="s">
+    <row r="39" spans="1:3" ht="15">
+      <c r="A39" s="15" t="s">
         <v>160</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="15" t="s">
         <v>161</v>
       </c>
-      <c r="C39" s="11" t="s">
+      <c r="C39" s="12" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="315">
-      <c r="A40" t="s">
+    <row r="40" spans="1:3" ht="15">
+      <c r="A40" s="15" t="s">
         <v>163</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="15" t="s">
         <v>164</v>
       </c>
-      <c r="C40" s="11" t="s">
+      <c r="C40" s="12" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="210">
-      <c r="A41" t="s">
+    <row r="41" spans="1:3" ht="15">
+      <c r="A41" s="15" t="s">
         <v>166</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="15" t="s">
         <v>167</v>
       </c>
-      <c r="C41" s="11" t="s">
+      <c r="C41" s="12" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="225">
-      <c r="A42" t="s">
+    <row r="42" spans="1:3" ht="15">
+      <c r="A42" s="15" t="s">
         <v>169</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="15" t="s">
         <v>170</v>
       </c>
-      <c r="C42" s="11" t="s">
+      <c r="C42" s="12" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="315">
-      <c r="A43" t="s">
+    <row r="43" spans="1:3" ht="15">
+      <c r="A43" s="15" t="s">
         <v>172</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="15" t="s">
         <v>173</v>
       </c>
-      <c r="C43" s="11" t="s">
+      <c r="C43" s="12" t="s">
         <v>174</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Working on Sprint 2.
</commit_message>
<xml_diff>
--- a/Team03Report.xlsx
+++ b/Team03Report.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
   <workbookPr date1904="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="17475" windowHeight="7380" tabRatio="819" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="-20" windowWidth="28800" windowHeight="17460" tabRatio="819" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,6 @@
     <sheet name="Stories" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="124519" concurrentCalc="0"/>
-  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="188">
   <si>
     <t>Initials</t>
   </si>
@@ -588,17 +587,20 @@
   </si>
   <si>
     <t>In progress</t>
+  </si>
+  <si>
+    <t>30 mins</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="m/d"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -658,9 +660,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -698,11 +704,15 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="10">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -784,7 +794,14 @@
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="1"/>
-  <c:style val="18"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
@@ -808,7 +825,13 @@
             <c:size val="4"/>
           </c:marker>
           <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
             <c:showBubbleSize val="1"/>
+            <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
             <c:numRef>
@@ -817,10 +840,13 @@
                 <c:formatCode>m/d</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>40946</c:v>
+                  <c:v>40946.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40966</c:v>
+                  <c:v>40966.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40982.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -832,28 +858,42 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>16</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12</c:v>
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="1"/>
         </c:ser>
-        <c:dLbls/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="54927744"/>
-        <c:axId val="54929280"/>
+        <c:smooth val="0"/>
+        <c:axId val="2105739752"/>
+        <c:axId val="2105736520"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="54927744"/>
+        <c:axId val="2105739752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="m/d" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:ln w="9360">
@@ -863,17 +903,18 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="54929280"/>
+        <c:crossAx val="2105736520"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="54929280"/>
+        <c:axId val="2105736520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -886,6 +927,8 @@
           </c:spPr>
         </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:ln w="9360">
@@ -895,8 +938,8 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="54927744"/>
-        <c:crossesAt val="0"/>
+        <c:crossAx val="2105739752"/>
+        <c:crossesAt val="0.0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
@@ -920,7 +963,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1" l="0.75000000000000011" r="0.75000000000000011" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1282,14 +1325,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
@@ -1366,16 +1409,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C9" sqref="B8:C9"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="5" max="5" width="18.25" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1">
@@ -1395,7 +1438,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="38.25">
+    <row r="2" spans="1:5" ht="39">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1412,7 +1455,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="38.25">
+    <row r="3" spans="1:5" ht="39">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1430,6 +1473,9 @@
       </c>
     </row>
     <row r="4" spans="1:5">
+      <c r="A4">
+        <v>2</v>
+      </c>
       <c r="B4" t="s">
         <v>27</v>
       </c>
@@ -1440,10 +1486,13 @@
         <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="5" spans="1:5">
+      <c r="A5">
+        <v>2</v>
+      </c>
       <c r="B5" t="s">
         <v>29</v>
       </c>
@@ -1454,7 +1503,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1492,6 +1541,9 @@
       </c>
     </row>
     <row r="8" spans="1:5">
+      <c r="A8">
+        <v>2</v>
+      </c>
       <c r="B8" t="s">
         <v>35</v>
       </c>
@@ -1502,10 +1554,13 @@
         <v>5</v>
       </c>
       <c r="E8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="9" spans="1:5">
+      <c r="A9">
+        <v>2</v>
+      </c>
       <c r="B9" t="s">
         <v>37</v>
       </c>
@@ -1520,11 +1575,20 @@
       </c>
     </row>
     <row r="10" spans="1:5">
+      <c r="A10">
+        <v>3</v>
+      </c>
       <c r="B10" t="s">
         <v>39</v>
       </c>
       <c r="C10" t="s">
         <v>40</v>
+      </c>
+      <c r="D10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -1568,11 +1632,20 @@
       </c>
     </row>
     <row r="16" spans="1:5">
+      <c r="A16">
+        <v>3</v>
+      </c>
       <c r="B16" t="s">
         <v>51</v>
       </c>
       <c r="C16" t="s">
         <v>52</v>
+      </c>
+      <c r="D16" t="s">
+        <v>5</v>
+      </c>
+      <c r="E16" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="17" spans="2:3">
@@ -1595,17 +1668,17 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="8.75" style="4"/>
-    <col min="6" max="6" width="8.75" style="5"/>
+    <col min="1" max="1" width="8.7109375" style="4"/>
+    <col min="6" max="6" width="8.7109375" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1">
@@ -1656,6 +1729,26 @@
         <v>180</v>
       </c>
       <c r="F3" s="5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="4">
+        <v>40982</v>
+      </c>
+      <c r="B4">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>800</v>
+      </c>
+      <c r="E4">
+        <v>390</v>
+      </c>
+      <c r="F4" s="5">
         <v>30</v>
       </c>
     </row>
@@ -1672,20 +1765,20 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="8.75" style="3"/>
-    <col min="9" max="9" width="8.75" style="4"/>
+    <col min="2" max="2" width="8.7109375" style="3"/>
+    <col min="9" max="9" width="8.7109375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="25.5">
+    <row r="1" spans="1:9" ht="26">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -1714,7 +1807,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="38.25">
+    <row r="2" spans="1:9" ht="39">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -1743,7 +1836,7 @@
         <v>40967</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="38.25">
+    <row r="3" spans="1:9" ht="39">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -1772,7 +1865,7 @@
         <v>40967</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="38.25">
+    <row r="4" spans="1:9" ht="39">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -1801,7 +1894,7 @@
         <v>40967</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="38.25">
+    <row r="5" spans="1:9" ht="39">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -1830,33 +1923,33 @@
         <v>40967</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="25.5">
+    <row r="14" spans="1:9" ht="26">
       <c r="B14" s="8" t="s">
         <v>71</v>
       </c>
       <c r="I14"/>
     </row>
-    <row r="15" spans="1:9" ht="153">
+    <row r="15" spans="1:9" ht="156">
       <c r="B15" s="11" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="25.5">
+    <row r="16" spans="1:9" ht="26">
       <c r="B16" s="8" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="17" spans="2:2" ht="38.25">
+    <row r="17" spans="2:2" ht="39">
       <c r="B17" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="2:2" ht="38.25">
+    <row r="18" spans="2:2" ht="39">
       <c r="B18" s="3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="19" spans="2:2" ht="216.75">
+    <row r="19" spans="2:2" ht="208">
       <c r="B19" s="11" t="s">
         <v>176</v>
       </c>
@@ -1866,19 +1959,19 @@
         <v>75</v>
       </c>
     </row>
-    <row r="21" spans="2:2" ht="63.75">
+    <row r="21" spans="2:2" ht="52">
       <c r="B21" s="3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="22" spans="2:2" ht="165.75">
+    <row r="22" spans="2:2" ht="169">
       <c r="B22" s="11" t="s">
         <v>177</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1888,19 +1981,19 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="25.5">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -1940,13 +2033,22 @@
         <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="E2" t="s">
         <v>66</v>
       </c>
       <c r="F2" t="s">
         <v>183</v>
+      </c>
+      <c r="G2" t="s">
+        <v>66</v>
+      </c>
+      <c r="H2" t="s">
+        <v>183</v>
+      </c>
+      <c r="I2" s="17">
+        <v>40982</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -1960,13 +2062,22 @@
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="E3" t="s">
         <v>66</v>
       </c>
       <c r="F3" t="s">
         <v>183</v>
+      </c>
+      <c r="G3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H3" t="s">
+        <v>183</v>
+      </c>
+      <c r="I3" s="17">
+        <v>40982</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -1980,13 +2091,22 @@
         <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="E4" t="s">
         <v>68</v>
       </c>
       <c r="F4" t="s">
         <v>183</v>
+      </c>
+      <c r="G4" t="s">
+        <v>68</v>
+      </c>
+      <c r="H4" t="s">
+        <v>187</v>
+      </c>
+      <c r="I4" s="17">
+        <v>40982</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -2007,6 +2127,54 @@
       </c>
       <c r="F5" t="s">
         <v>183</v>
+      </c>
+      <c r="I5" s="17">
+        <v>40982</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="B9" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="39">
+      <c r="B10" s="11" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="B11" s="8" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="B12" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="B13" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="52">
+      <c r="B14" s="11" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="B15" s="8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="B16" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" ht="39">
+      <c r="B17" s="11" t="s">
+        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -2021,16 +2189,16 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="25.5">
+    <row r="1" spans="1:9" ht="26">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -2071,16 +2239,16 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="25.5">
+    <row r="1" spans="1:9" ht="26">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -2121,18 +2289,18 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="2" width="8.75" style="15"/>
-    <col min="3" max="3" width="8.75" style="16"/>
-    <col min="4" max="16384" width="8.75" style="15"/>
+    <col min="1" max="2" width="8.7109375" style="15"/>
+    <col min="3" max="3" width="8.7109375" style="16"/>
+    <col min="4" max="16384" width="8.7109375" style="15"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="13" customFormat="1">
@@ -2146,7 +2314,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75">
+    <row r="2" spans="1:3" ht="15">
       <c r="A2" s="15" t="s">
         <v>35</v>
       </c>
@@ -2157,7 +2325,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.75">
+    <row r="3" spans="1:3" ht="15">
       <c r="A3" s="15" t="s">
         <v>25</v>
       </c>
@@ -2168,7 +2336,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75">
+    <row r="4" spans="1:3" ht="15">
       <c r="A4" s="15" t="s">
         <v>22</v>
       </c>
@@ -2179,7 +2347,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.75">
+    <row r="5" spans="1:3" ht="15">
       <c r="A5" s="15" t="s">
         <v>81</v>
       </c>
@@ -2190,7 +2358,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.75">
+    <row r="6" spans="1:3" ht="15">
       <c r="A6" s="15" t="s">
         <v>31</v>
       </c>
@@ -2201,7 +2369,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.75">
+    <row r="7" spans="1:3" ht="15">
       <c r="A7" s="15" t="s">
         <v>27</v>
       </c>
@@ -2212,7 +2380,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15.75">
+    <row r="8" spans="1:3" ht="15">
       <c r="A8" s="15" t="s">
         <v>33</v>
       </c>
@@ -2223,7 +2391,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15.75">
+    <row r="9" spans="1:3" ht="15">
       <c r="A9" s="15" t="s">
         <v>37</v>
       </c>
@@ -2234,7 +2402,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15.75">
+    <row r="10" spans="1:3" ht="15">
       <c r="A10" s="15" t="s">
         <v>89</v>
       </c>
@@ -2245,7 +2413,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15.75">
+    <row r="11" spans="1:3" ht="15">
       <c r="A11" s="15" t="s">
         <v>39</v>
       </c>
@@ -2256,7 +2424,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15.75">
+    <row r="12" spans="1:3" ht="15">
       <c r="A12" s="15" t="s">
         <v>29</v>
       </c>
@@ -2267,7 +2435,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15.75">
+    <row r="13" spans="1:3" ht="15">
       <c r="A13" s="15" t="s">
         <v>41</v>
       </c>
@@ -2278,7 +2446,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="15.75">
+    <row r="14" spans="1:3" ht="15">
       <c r="A14" s="15" t="s">
         <v>43</v>
       </c>
@@ -2289,7 +2457,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15.75">
+    <row r="15" spans="1:3" ht="15">
       <c r="A15" s="15" t="s">
         <v>97</v>
       </c>
@@ -2300,7 +2468,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15.75">
+    <row r="16" spans="1:3" ht="15">
       <c r="A16" s="15" t="s">
         <v>100</v>
       </c>
@@ -2311,7 +2479,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15.75">
+    <row r="17" spans="1:3" ht="15">
       <c r="A17" s="15" t="s">
         <v>103</v>
       </c>
@@ -2322,7 +2490,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15.75">
+    <row r="18" spans="1:3" ht="15">
       <c r="A18" s="15" t="s">
         <v>45</v>
       </c>
@@ -2333,7 +2501,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15.75">
+    <row r="19" spans="1:3" ht="15">
       <c r="A19" s="15" t="s">
         <v>47</v>
       </c>
@@ -2344,7 +2512,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15.75">
+    <row r="20" spans="1:3" ht="15">
       <c r="A20" s="15" t="s">
         <v>108</v>
       </c>
@@ -2355,7 +2523,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15.75">
+    <row r="21" spans="1:3" ht="15">
       <c r="A21" s="15" t="s">
         <v>111</v>
       </c>
@@ -2366,7 +2534,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="15.75">
+    <row r="22" spans="1:3" ht="15">
       <c r="A22" s="15" t="s">
         <v>49</v>
       </c>
@@ -2377,7 +2545,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="15.75">
+    <row r="23" spans="1:3" ht="15">
       <c r="A23" s="15" t="s">
         <v>51</v>
       </c>
@@ -2388,7 +2556,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="15.75">
+    <row r="24" spans="1:3" ht="15">
       <c r="A24" s="15" t="s">
         <v>116</v>
       </c>
@@ -2399,7 +2567,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="15.75">
+    <row r="25" spans="1:3" ht="15">
       <c r="A25" s="15" t="s">
         <v>119</v>
       </c>
@@ -2410,7 +2578,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="15.75">
+    <row r="26" spans="1:3" ht="15">
       <c r="A26" s="15" t="s">
         <v>122</v>
       </c>
@@ -2421,7 +2589,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="15.75">
+    <row r="27" spans="1:3" ht="15">
       <c r="A27" s="15" t="s">
         <v>125</v>
       </c>
@@ -2432,7 +2600,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15.75">
+    <row r="28" spans="1:3" ht="15">
       <c r="A28" s="15" t="s">
         <v>53</v>
       </c>
@@ -2443,7 +2611,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="15.75">
+    <row r="29" spans="1:3" ht="15">
       <c r="A29" s="15" t="s">
         <v>130</v>
       </c>
@@ -2454,7 +2622,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15.75">
+    <row r="30" spans="1:3" ht="15">
       <c r="A30" s="15" t="s">
         <v>133</v>
       </c>
@@ -2465,7 +2633,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15.75">
+    <row r="31" spans="1:3" ht="15">
       <c r="A31" s="15" t="s">
         <v>136</v>
       </c>
@@ -2476,7 +2644,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="15.75">
+    <row r="32" spans="1:3" ht="15">
       <c r="A32" s="15" t="s">
         <v>139</v>
       </c>
@@ -2487,7 +2655,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15.75">
+    <row r="33" spans="1:3" ht="15">
       <c r="A33" s="15" t="s">
         <v>142</v>
       </c>
@@ -2498,7 +2666,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="15.75">
+    <row r="34" spans="1:3" ht="15">
       <c r="A34" s="15" t="s">
         <v>145</v>
       </c>
@@ -2509,7 +2677,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="15.75">
+    <row r="35" spans="1:3" ht="15">
       <c r="A35" s="15" t="s">
         <v>148</v>
       </c>
@@ -2520,7 +2688,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="15.75">
+    <row r="36" spans="1:3" ht="15">
       <c r="A36" s="15" t="s">
         <v>151</v>
       </c>
@@ -2531,7 +2699,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="15.75">
+    <row r="37" spans="1:3" ht="15">
       <c r="A37" s="15" t="s">
         <v>154</v>
       </c>
@@ -2542,7 +2710,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="15.75">
+    <row r="38" spans="1:3" ht="15">
       <c r="A38" s="15" t="s">
         <v>157</v>
       </c>
@@ -2553,7 +2721,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="15.75">
+    <row r="39" spans="1:3" ht="15">
       <c r="A39" s="15" t="s">
         <v>160</v>
       </c>
@@ -2564,7 +2732,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="15.75">
+    <row r="40" spans="1:3" ht="15">
       <c r="A40" s="15" t="s">
         <v>163</v>
       </c>
@@ -2575,7 +2743,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="15.75">
+    <row r="41" spans="1:3" ht="15">
       <c r="A41" s="15" t="s">
         <v>166</v>
       </c>
@@ -2586,7 +2754,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="15.75">
+    <row r="42" spans="1:3" ht="15">
       <c r="A42" s="15" t="s">
         <v>169</v>
       </c>
@@ -2597,7 +2765,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="15.75">
+    <row r="43" spans="1:3" ht="15">
       <c r="A43" s="15" t="s">
         <v>172</v>
       </c>

</xml_diff>

<commit_message>
Wrapping up Sprint 2.
</commit_message>
<xml_diff>
--- a/Team03Report.xlsx
+++ b/Team03Report.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
   <workbookPr date1904="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-20" windowWidth="28800" windowHeight="17460" tabRatio="819" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="-20" windowWidth="28800" windowHeight="17460" tabRatio="819" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="188">
   <si>
     <t>Initials</t>
   </si>
@@ -586,10 +586,10 @@
     <t>10 LOC</t>
   </si>
   <si>
-    <t>In progress</t>
-  </si>
-  <si>
     <t>30 mins</t>
+  </si>
+  <si>
+    <t>Unique ID's</t>
   </si>
 </sst>
 </file>
@@ -660,9 +660,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="10">
+  <cellStyleXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -704,7 +706,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="10">
+  <cellStyles count="12">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -713,6 +715,8 @@
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -881,11 +885,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2105739752"/>
-        <c:axId val="2105736520"/>
+        <c:axId val="2100107768"/>
+        <c:axId val="2100111032"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="2105739752"/>
+        <c:axId val="2100107768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -903,14 +907,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="2105736520"/>
+        <c:crossAx val="2100111032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="2105736520"/>
+        <c:axId val="2100111032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -938,7 +942,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="2105739752"/>
+        <c:crossAx val="2100107768"/>
         <c:crossesAt val="0.0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1413,11 +1417,12 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="C12" sqref="C10:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
+    <col min="3" max="3" width="28.7109375" customWidth="1"/>
     <col min="5" max="5" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1438,7 +1443,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="39">
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1455,7 +1460,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="39">
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1571,7 +1576,7 @@
         <v>5</v>
       </c>
       <c r="E9" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1592,19 +1597,37 @@
       </c>
     </row>
     <row r="11" spans="1:5">
+      <c r="A11">
+        <v>3</v>
+      </c>
       <c r="B11" t="s">
         <v>41</v>
       </c>
       <c r="C11" t="s">
         <v>42</v>
       </c>
+      <c r="D11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="12" spans="1:5">
+      <c r="A12">
+        <v>3</v>
+      </c>
       <c r="B12" t="s">
         <v>43</v>
       </c>
       <c r="C12" t="s">
         <v>44</v>
+      </c>
+      <c r="D12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -1982,10 +2005,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -2103,7 +2126,7 @@
         <v>68</v>
       </c>
       <c r="H4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="I4" s="17">
         <v>40982</v>
@@ -2120,13 +2143,19 @@
         <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="E5" t="s">
         <v>66</v>
       </c>
       <c r="F5" t="s">
         <v>183</v>
+      </c>
+      <c r="G5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H5" t="s">
+        <v>186</v>
       </c>
       <c r="I5" s="17">
         <v>40982</v>
@@ -2167,13 +2196,8 @@
         <v>75</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
-      <c r="B16" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" ht="39">
-      <c r="B17" s="11" t="s">
+    <row r="16" spans="1:9" ht="39">
+      <c r="B16" s="11" t="s">
         <v>177</v>
       </c>
     </row>
@@ -2190,10 +2214,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -2225,6 +2249,86 @@
       </c>
       <c r="I1" s="9" t="s">
         <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>179</v>
+      </c>
+      <c r="E2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>179</v>
+      </c>
+      <c r="E3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F3" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>179</v>
+      </c>
+      <c r="E4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F4" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" t="s">
+        <v>187</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>179</v>
+      </c>
+      <c r="E5" t="s">
+        <v>66</v>
+      </c>
+      <c r="F5" t="s">
+        <v>183</v>
       </c>
     </row>
   </sheetData>
@@ -2292,7 +2396,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
ZD Sprint 3 Work.
</commit_message>
<xml_diff>
--- a/Team03Report.xlsx
+++ b/Team03Report.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
   <workbookPr date1904="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-20" windowWidth="28800" windowHeight="17460" tabRatio="819" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="-20" windowWidth="28800" windowHeight="17460" tabRatio="819" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="188">
   <si>
     <t>Initials</t>
   </si>
@@ -660,9 +660,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="12">
+  <cellStyleXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -706,7 +714,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="12">
+  <cellStyles count="20">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -717,6 +725,14 @@
     <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -852,6 +868,9 @@
                 <c:pt idx="2">
                   <c:v>40982.0</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>41013.0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -870,6 +889,9 @@
                 <c:pt idx="2">
                   <c:v>8.0</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -885,11 +907,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2100107768"/>
-        <c:axId val="2100111032"/>
+        <c:axId val="2075784680"/>
+        <c:axId val="2048066344"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="2100107768"/>
+        <c:axId val="2075784680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -907,14 +929,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="2100111032"/>
+        <c:crossAx val="2048066344"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="2100111032"/>
+        <c:axId val="2048066344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -942,7 +964,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="2100107768"/>
+        <c:crossAx val="2075784680"/>
         <c:crossesAt val="0.0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1417,7 +1439,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C12" sqref="C10:C12"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -1593,7 +1615,7 @@
         <v>5</v>
       </c>
       <c r="E10" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -1610,7 +1632,7 @@
         <v>10</v>
       </c>
       <c r="E11" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -1627,31 +1649,58 @@
         <v>10</v>
       </c>
       <c r="E12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="13" spans="1:5">
+      <c r="A13">
+        <v>4</v>
+      </c>
       <c r="B13" t="s">
         <v>45</v>
       </c>
       <c r="C13" t="s">
         <v>46</v>
       </c>
+      <c r="D13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="14" spans="1:5">
+      <c r="A14">
+        <v>4</v>
+      </c>
       <c r="B14" t="s">
         <v>47</v>
       </c>
       <c r="C14" t="s">
         <v>48</v>
       </c>
+      <c r="D14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="15" spans="1:5">
+      <c r="A15">
+        <v>4</v>
+      </c>
       <c r="B15" t="s">
         <v>49</v>
       </c>
       <c r="C15" t="s">
         <v>50</v>
+      </c>
+      <c r="D15" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -1668,15 +1717,24 @@
         <v>5</v>
       </c>
       <c r="E16" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17">
+        <v>4</v>
+      </c>
       <c r="B17" t="s">
         <v>53</v>
       </c>
       <c r="C17" t="s">
         <v>54</v>
+      </c>
+      <c r="D17" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" t="s">
+        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -1692,10 +1750,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -1772,6 +1830,26 @@
         <v>390</v>
       </c>
       <c r="F4" s="5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="4">
+        <v>41013</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>1000</v>
+      </c>
+      <c r="E5">
+        <v>630</v>
+      </c>
+      <c r="F5" s="5">
         <v>30</v>
       </c>
     </row>
@@ -2007,8 +2085,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B16" sqref="B9:B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -2214,15 +2292,18 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="29.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="26">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -2270,6 +2351,15 @@
       <c r="F2" t="s">
         <v>183</v>
       </c>
+      <c r="G2" t="s">
+        <v>66</v>
+      </c>
+      <c r="H2" t="s">
+        <v>183</v>
+      </c>
+      <c r="I2" s="17">
+        <v>41003</v>
+      </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
@@ -2290,6 +2380,15 @@
       <c r="F3" t="s">
         <v>183</v>
       </c>
+      <c r="G3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H3" t="s">
+        <v>183</v>
+      </c>
+      <c r="I3" s="17">
+        <v>41003</v>
+      </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
@@ -2310,6 +2409,15 @@
       <c r="F4" t="s">
         <v>183</v>
       </c>
+      <c r="G4" t="s">
+        <v>66</v>
+      </c>
+      <c r="H4" t="s">
+        <v>183</v>
+      </c>
+      <c r="I4" s="17">
+        <v>41003</v>
+      </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
@@ -2329,6 +2437,55 @@
       </c>
       <c r="F5" t="s">
         <v>183</v>
+      </c>
+      <c r="G5" t="s">
+        <v>66</v>
+      </c>
+      <c r="H5" t="s">
+        <v>183</v>
+      </c>
+      <c r="I5" s="17">
+        <v>41003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="B8" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="39">
+      <c r="B9" s="11" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="B10" s="8" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="B11" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="B12" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="52">
+      <c r="B13" s="11" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="B14" s="8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="39">
+      <c r="B15" s="11" t="s">
+        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -2344,10 +2501,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -2379,6 +2536,86 @@
       </c>
       <c r="I1" s="9" t="s">
         <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>179</v>
+      </c>
+      <c r="E2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>179</v>
+      </c>
+      <c r="E3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F3" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>179</v>
+      </c>
+      <c r="E4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F4" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>179</v>
+      </c>
+      <c r="E5" t="s">
+        <v>66</v>
+      </c>
+      <c r="F5" t="s">
+        <v>183</v>
       </c>
     </row>
   </sheetData>
@@ -2396,8 +2633,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView topLeftCell="A2" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>

</xml_diff>